<commit_message>
Fixing issues in wildfire activity stats files
</commit_message>
<xml_diff>
--- a/Resources/CAL_FireStats/2008-wildfire-activity-stats.xlsx
+++ b/Resources/CAL_FireStats/2008-wildfire-activity-stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16c6a743d20dd4b9/Documents/^M PERSONLIG/^M MAAL/DABC/Working/Projects/Project3/Fire-Analysis/Resources/CAL_FireStats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16c6a743d20dd4b9/Documents/^M PERSONLIG/^M MAAL/DABC/Working/Projects/Project3/Fire-Analysis/Resources/UniformXLSXs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="11_322FEBFA675BCE483F4C7FB221F65502CCEF4F36" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{567DAC55-A979-47CC-8531-33839FF05AAF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A752AF3-C7B3-4FB2-8445-57204BD6FDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1545" yWindow="825" windowWidth="27255" windowHeight="14760" firstSheet="43" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>